<commit_message>
28 de octubre 2
</commit_message>
<xml_diff>
--- a/SEMANA 8/28 de octubre.xlsx
+++ b/SEMANA 8/28 de octubre.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kick\Desktop\MATEMATICAS FINANCIERA\prueba\MF\SEMANA 8\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3D78CC3-F886-494E-8C98-07BED52FD219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D953DE9-039D-4917-A77C-C63A24F303CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9912" yWindow="24" windowWidth="13068" windowHeight="12312" firstSheet="20" activeTab="21" xr2:uid="{E581A421-F443-4CC0-8F82-30A63A821E48}"/>
+    <workbookView xWindow="10104" yWindow="24" windowWidth="12876" windowHeight="12312" firstSheet="21" activeTab="22" xr2:uid="{E581A421-F443-4CC0-8F82-30A63A821E48}"/>
   </bookViews>
   <sheets>
     <sheet name="Interes compuesto" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,8 @@
     <sheet name="TIEMPO" sheetId="19" r:id="rId19"/>
     <sheet name="Ejercicio 1 tiempo logaritmo" sheetId="20" r:id="rId20"/>
     <sheet name="Tiempo logaritmo Caso 2" sheetId="21" r:id="rId21"/>
-    <sheet name="Hoja1" sheetId="22" r:id="rId22"/>
+    <sheet name="EJERCICIO REPASO" sheetId="22" r:id="rId22"/>
+    <sheet name="Tasa de interes" sheetId="23" r:id="rId23"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="120">
   <si>
     <t>Interes compuesto</t>
   </si>
@@ -401,7 +402,19 @@
     <t>EJERCICIO 8</t>
   </si>
   <si>
-    <t>prue</t>
+    <t>TASA DE INTERES</t>
+  </si>
+  <si>
+    <t>anual</t>
+  </si>
+  <si>
+    <t>semestral</t>
+  </si>
+  <si>
+    <t>mensualmente</t>
+  </si>
+  <si>
+    <t>NP</t>
   </si>
 </sst>
 </file>
@@ -527,7 +540,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="89">
+  <borders count="90">
     <border>
       <left/>
       <right/>
@@ -1612,6 +1625,21 @@
       </top>
       <bottom style="thin">
         <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1621,7 +1649,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="284">
+  <cellXfs count="301">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1964,6 +1992,27 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="87" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="86" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="89" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="67" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="67" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="68" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Moneda" xfId="2" builtinId="4"/>
@@ -4255,10 +4304,10 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFC50662-5A60-464F-BC85-7B2374E70255}">
-  <dimension ref="C1:G79"/>
+  <dimension ref="C1:E79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4266,26 +4315,26 @@
     <col min="5" max="5" width="14.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C1" s="234" t="s">
         <v>109</v>
       </c>
       <c r="D1" s="234"/>
       <c r="E1" s="234"/>
     </row>
-    <row r="2" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C2" s="235" t="s">
         <v>90</v>
       </c>
       <c r="D2" s="230"/>
       <c r="E2" s="236"/>
     </row>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C3" s="224"/>
       <c r="D3" s="195"/>
       <c r="E3" s="225"/>
     </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C4" s="211" t="s">
         <v>33</v>
       </c>
@@ -4296,7 +4345,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C5" s="212" t="s">
         <v>9</v>
       </c>
@@ -4307,7 +4356,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C6" s="212" t="s">
         <v>10</v>
       </c>
@@ -4319,7 +4368,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C7" s="226"/>
       <c r="D7" s="22" t="s">
         <v>13</v>
@@ -4328,7 +4377,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C8" s="226"/>
       <c r="D8" s="213" t="s">
         <v>102</v>
@@ -4338,27 +4387,24 @@
         <v>110.40962404966885</v>
       </c>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C9" s="227"/>
       <c r="D9" s="195"/>
       <c r="E9" s="225"/>
-      <c r="G9" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C13" s="235" t="s">
         <v>107</v>
       </c>
       <c r="D13" s="230"/>
       <c r="E13" s="236"/>
     </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C14" s="257"/>
       <c r="D14" s="258"/>
       <c r="E14" s="259"/>
     </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C15" s="211" t="s">
         <v>33</v>
       </c>
@@ -4369,7 +4415,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C16" s="212" t="s">
         <v>9</v>
       </c>
@@ -4853,6 +4899,152 @@
     <mergeCell ref="C23:E23"/>
     <mergeCell ref="C32:E32"/>
     <mergeCell ref="C42:E42"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{699F2A28-63DF-4A35-9854-8A9CF575719D}">
+  <dimension ref="C1:H22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" customWidth="1"/>
+    <col min="8" max="8" width="15" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C1" s="247" t="s">
+        <v>115</v>
+      </c>
+      <c r="D1" s="248"/>
+      <c r="E1" s="248"/>
+      <c r="F1" s="248"/>
+      <c r="G1" s="248"/>
+      <c r="H1" s="286"/>
+    </row>
+    <row r="2" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C2" s="147" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E2" s="287">
+        <v>50000</v>
+      </c>
+      <c r="F2" s="294"/>
+      <c r="G2" s="294"/>
+      <c r="H2" s="295"/>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C3" s="292" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="288">
+        <v>15000</v>
+      </c>
+      <c r="F3" s="296"/>
+      <c r="G3" s="297"/>
+      <c r="H3" s="298"/>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C4" s="148" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="5">
+        <v>5</v>
+      </c>
+      <c r="F4" s="291">
+        <f>E4*2</f>
+        <v>10</v>
+      </c>
+      <c r="G4" s="291">
+        <f>F4*2</f>
+        <v>20</v>
+      </c>
+      <c r="H4" s="290">
+        <f>E4*12</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C5" s="299"/>
+      <c r="D5" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F5" s="299"/>
+      <c r="G5" s="299"/>
+      <c r="H5" s="295"/>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C6" s="300"/>
+      <c r="D6" s="50" t="s">
+        <v>116</v>
+      </c>
+      <c r="E6" s="57"/>
+      <c r="F6" s="292" t="s">
+        <v>117</v>
+      </c>
+      <c r="G6" s="292" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C7" s="296"/>
+      <c r="D7" s="297"/>
+      <c r="E7" s="298"/>
+      <c r="F7" s="300"/>
+      <c r="G7" s="300"/>
+      <c r="H7" s="298"/>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C8" s="8"/>
+      <c r="D8" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="289">
+        <f>RATE(E4,,-$E$3,$E$2)</f>
+        <v>0.27225963653939206</v>
+      </c>
+      <c r="F8" s="284">
+        <f>RATE(F4,,-$E$3,$E$2)</f>
+        <v>0.12794487300549931</v>
+      </c>
+      <c r="G8" s="284">
+        <f>RATE(G4,,-$E$3,$E$2)</f>
+        <v>6.204749093696342E-2</v>
+      </c>
+      <c r="H8" s="285">
+        <f>RATE(H4,,-$E$3,$E$2)</f>
+        <v>2.0268893268145939E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="6:6" x14ac:dyDescent="0.3">
+      <c r="F22" s="293"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>